<commit_message>
testing done for sample_gear_shifting
</commit_message>
<xml_diff>
--- a/new_MFC/template/sample.xlsx
+++ b/new_MFC/template/sample.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apps\new_MFC\new_MFC\template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9435" activeTab="1"/>
   </bookViews>
@@ -13,8 +18,8 @@
     <sheet name="time_series" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -173,8 +178,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,27 +495,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -521,7 +526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -532,7 +537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -549,21 +554,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
     <col min="3" max="3" width="58.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -571,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -582,7 +587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -594,20 +599,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -615,7 +620,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -630,16 +635,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -653,7 +658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -661,7 +666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -669,7 +674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -677,7 +682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -685,7 +690,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -693,7 +698,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -701,7 +706,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -709,7 +714,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -717,7 +722,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -725,7 +730,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -733,7 +738,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -741,7 +746,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -749,7 +754,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -757,7 +762,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -765,7 +770,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -773,7 +778,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -781,7 +786,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -789,7 +794,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -797,7 +802,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -805,7 +810,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -813,7 +818,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>

</xml_diff>